<commit_message>
Implemented most of the audio
Still needs some tweaking and testing, but the first pass is fairly
good.
</commit_message>
<xml_diff>
--- a/Assets/Audio/Audio master spreadsheet.xlsx
+++ b/Assets/Audio/Audio master spreadsheet.xlsx
@@ -42,9 +42,6 @@
     <t>TTT fail to place piece</t>
   </si>
   <si>
-    <t>TTT move cursor</t>
-  </si>
-  <si>
     <t>TTT transition to SW</t>
   </si>
   <si>
@@ -154,13 +151,16 @@
   </si>
   <si>
     <t>SW engine throttle down</t>
+  </si>
+  <si>
+    <t>TTT move cursor into edge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +183,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +206,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,20 +249,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,7 +568,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,8 +576,8 @@
     <col min="1" max="1" width="26.109375" customWidth="1"/>
     <col min="2" max="2" width="32.109375" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="57.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,217 +592,217 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D10" s="4"/>
       <c r="E10" s="2"/>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
       <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
       <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D12" s="4"/>
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="2"/>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>

</xml_diff>